<commit_message>
task 4, 5 complete. task 6 almost done
</commit_message>
<xml_diff>
--- a/Game Business Studies/task 5/Diavolo3_Tasks.xlsx
+++ b/Game Business Studies/task 5/Diavolo3_Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s231135\GitHub\Robert-2\Game Business Studies\task 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30308628-6A82-4CBA-B885-D9BF9B8FB282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E813A358-E208-40F0-A3CB-7F8D86C3A52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{04AC3E2D-6759-42B0-BB9D-DEFE897D259F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{04AC3E2D-6759-42B0-BB9D-DEFE897D259F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>Character Controller</t>
   </si>
@@ -88,12 +88,6 @@
     <t>Wilderness level</t>
   </si>
   <si>
-    <t>Mage model</t>
-  </si>
-  <si>
-    <t>Warrior model</t>
-  </si>
-  <si>
     <t>Wilderness props</t>
   </si>
   <si>
@@ -209,6 +203,15 @@
   </si>
   <si>
     <t>hello :D</t>
+  </si>
+  <si>
+    <t>Character Customisation</t>
+  </si>
+  <si>
+    <t>Character Customisation tests</t>
+  </si>
+  <si>
+    <t>Player models</t>
   </si>
 </sst>
 </file>
@@ -276,9 +279,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -316,7 +319,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -422,7 +425,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -564,7 +567,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -575,7 +578,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,22 +597,22 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -620,19 +623,19 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2">
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -646,10 +649,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -658,7 +661,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -672,19 +675,19 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -698,19 +701,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -724,19 +727,19 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="2">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -750,15 +753,21 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7">
         <v>5</v>
       </c>
     </row>
@@ -770,7 +779,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2">
         <v>5</v>
@@ -790,13 +799,13 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F9" s="2">
         <v>5</v>
@@ -813,10 +822,10 @@
         <v>27</v>
       </c>
       <c r="D10" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2">
         <v>5</v>
@@ -830,13 +839,13 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F11" s="2">
         <v>3</v>
@@ -850,13 +859,13 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F12" s="2">
         <v>3</v>
@@ -870,13 +879,13 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F13" s="2">
         <v>3</v>
@@ -884,19 +893,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F14" s="2">
         <v>3</v>
@@ -904,21 +913,33 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="2">
+        <v>10</v>
+      </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D16" s="2">
         <v>5</v>
@@ -926,15 +947,15 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D17" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D18" s="2">
         <v>10</v>
@@ -942,18 +963,18 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -961,43 +982,35 @@
         <v>45</v>
       </c>
       <c r="D21" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23">
         <f>SUM(B2:B19)</f>
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D23">
-        <f>SUM(D2:D22)</f>
-        <v>130</v>
+        <f>SUM(D2:D21)</f>
+        <v>135</v>
       </c>
       <c r="F23">
         <f>SUM(F2:F19)</f>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="H23">
         <f>SUM(H2:H19)</f>
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="1048576" spans="16384:16384" x14ac:dyDescent="0.25">
       <c r="XFD1048576" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>